<commit_message>
Add headers to Excel output
</commit_message>
<xml_diff>
--- a/Service Overview.xlsx
+++ b/Service Overview.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:Q10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -424,123 +424,99 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
+          <t>PORT</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>MICT SERVICE NAME</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>SERVICE NAME</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
           <t>SERVICE DESC</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>FIRST VESSEL ON LIST</t>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>ROUTE</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>LEAD SL</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>SAILING FREQ</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>PARTICIPANTS</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>VESSEL OPERATOR</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t># OF VESSELS</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t># OF VESSELS PER ROW COUNT</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>WEEKLY CAPACITY</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>SHIPS USED</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>PORT ROTATION</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>ALT SRVC CD</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
+          <t>VESSEL SIZE</t>
+        </is>
+      </c>
+      <c r="Q1" t="inlineStr">
+        <is>
+          <t>VESSEL_NAME</t>
         </is>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>CNC - China-South East Asia service (KCS)</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>CNC</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>COSCO - China-Philippines Express service (CNP 2)</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>COSCO SHIPPING Lines</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>CNC - Japan-Straits Express (JSX / JPX)</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>CNC</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>CNC - China-Philippines service (Bohai-Manila Express - BMX)</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>CNC</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>COSCO / TS Lines / RCL / CMA CGM / UniFeeder/ KMTC - India East Coast Express</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>CMA CGM</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>CNC - China-South Korea-Thailand-Philippines-Vietnam service (CSE)</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>CNC</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>Evergreen - China-Taiwan-Philippines service (KTP)</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>Evergreen Line</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>Asean Seas Line / Gold Star Line – China-Philippines service (NPX)</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>Asean Seas Line Co (ASL)</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>Asean Seas Line – China-Philippines service (NPX2)</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>Asean Seas Line Co (ASL)</t>
-        </is>
-      </c>
-    </row>
+    <row r="2"/>
+    <row r="3"/>
+    <row r="4"/>
+    <row r="5"/>
+    <row r="6"/>
+    <row r="7"/>
+    <row r="8"/>
+    <row r="9"/>
+    <row r="10"/>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>